<commit_message>
cambios en estatus eventos
</commit_message>
<xml_diff>
--- a/EmpManagement/Excel/gafete.xlsx
+++ b/EmpManagement/Excel/gafete.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\userf\source\repos\EmpManagement\EmpManagement\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A13DAB-48E1-463B-90FC-E3AF1DC3A9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFEC235-AC1C-43BF-8997-B67A2F624D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9AD466DE-D675-454B-B321-B1406A6968E6}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="10890" xr2:uid="{9AD466DE-D675-454B-B321-B1406A6968E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,15 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>COMPAÑÍA PLÁSTICA INTERNACIONAL S.A. DE C.V</t>
   </si>
   <si>
-    <t>María del Socorro Navarro</t>
-  </si>
-  <si>
-    <t>OPERARÍA DE INYECCIÓN</t>
+    <t>Selma Sacbé Ramírez Peralta</t>
   </si>
 </sst>
 </file>
@@ -104,14 +101,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -810,12 +807,12 @@
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
@@ -824,16 +821,16 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>2</v>
+      <c r="B10" s="3" t="e">
+        <v>#N/A</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -876,13 +873,13 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="str">
+      <c r="B19" s="4" t="str">
         <f>B7</f>
         <v>COMPAÑÍA PLÁSTICA INTERNACIONAL S.A. DE C.V</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
@@ -893,16 +890,16 @@
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="str">
         <f>B9</f>
-        <v>María del Socorro Navarro</v>
+        <v>Selma Sacbé Ramírez Peralta</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="str">
+      <c r="B22" s="3" t="e">
         <f>B10</f>
-        <v>OPERARÍA DE INYECCIÓN</v>
+        <v>#N/A</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -945,13 +942,13 @@
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="str">
+      <c r="B31" s="4" t="str">
         <f>B19</f>
         <v>COMPAÑÍA PLÁSTICA INTERNACIONAL S.A. DE C.V</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -960,18 +957,18 @@
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="str">
+      <c r="B33" s="2" t="str">
         <f>B21</f>
-        <v>María del Socorro Navarro</v>
+        <v>Selma Sacbé Ramírez Peralta</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="str">
+      <c r="B34" s="3" t="e">
         <f>B22</f>
-        <v>OPERARÍA DE INYECCIÓN</v>
+        <v>#N/A</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>

</xml_diff>